<commit_message>
Upload formatted Wind Technical Details file
</commit_message>
<xml_diff>
--- a/data/example/Power_Wind_TechnicalDetails.xlsx
+++ b/data/example/Power_Wind_TechnicalDetails.xlsx
@@ -557,7 +557,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <tabColor rgb="00008080"/>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -599,9 +599,9 @@
     <col width="15.7109375" customWidth="1" min="23" max="23"/>
     <col width="15.7109375" customWidth="1" min="24" max="24"/>
     <col width="15.7109375" customWidth="1" min="25" max="25"/>
-    <col width="15.7109375" customWidth="1" min="26" max="26"/>
-    <col width="18.7109375" customWidth="1" min="27" max="27"/>
-    <col width="18.7109375" customWidth="1" min="28" max="28"/>
+    <col width="25.7109375" customWidth="1" min="26" max="26"/>
+    <col width="20.2109375" customWidth="1" min="27" max="27"/>
+    <col width="28.7109375" customWidth="1" min="28" max="28"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1058,17 +1058,17 @@
       </c>
       <c r="Z5" s="7" t="inlineStr">
         <is>
-          <t>Power Factor for the given Year</t>
+          <t>Power Factor for this unit, correcting for maintenance, terrain specifics, etc.</t>
         </is>
       </c>
       <c r="AA5" s="7" t="inlineStr">
         <is>
-          <t>Year</t>
+          <t>Year of the Yearly Production that is given</t>
         </is>
       </c>
       <c r="AB5" s="7" t="inlineStr">
         <is>
-          <t>Yearly production for calibration</t>
+          <t>Yearly production for calibration (i.e., used to calculate Power Factor if it's not specified yet)</t>
         </is>
       </c>
     </row>
@@ -1810,6 +1810,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>
+  <legacyDrawing r:id="anysvml"/>
 </worksheet>
 </file>
</xml_diff>